<commit_message>
import data for 2021.06
</commit_message>
<xml_diff>
--- a/databases/xlsx/import 2021.06 июнь/import 2021.06 июнь.xlsx
+++ b/databases/xlsx/import 2021.06 июнь/import 2021.06 июнь.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Корректировки показаний" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="516">
   <si>
     <t xml:space="preserve">ООО Будь здоров (Ригла)</t>
   </si>
@@ -2369,6 +2370,24 @@
   </si>
   <si>
     <t xml:space="preserve">корп.№1, Зоомагазин</t>
+  </si>
+  <si>
+    <t xml:space="preserve">№ счетчика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Примечание</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Корректные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НЕ корректные</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Предыдущие</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Текущие</t>
   </si>
 </sst>
 </file>
@@ -2569,7 +2588,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2578,14 +2597,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFDBB6"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFF5CE"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFF5CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDE8CB"/>
+        <bgColor rgb="FFFFF5CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAA95"/>
+        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -2676,7 +2707,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="88">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2945,10 +2976,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="9" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2977,11 +3004,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3015,7 +3090,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFF5CE"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -3031,12 +3106,12 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFDDE8CB"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFAA95"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFDBB6"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -3063,13 +3138,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G208"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A175" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F198" activeCellId="0" sqref="F198"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A181" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B172" activeCellId="0" sqref="B172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="24.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="24.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="92.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.41"/>
@@ -3077,7 +3152,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="42.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="138.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6093,10 +6168,10 @@
       <c r="C148" s="66" t="n">
         <v>2187</v>
       </c>
-      <c r="D148" s="67" t="n">
-        <v>1</v>
-      </c>
-      <c r="E148" s="68" t="s">
+      <c r="D148" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E148" s="67" t="s">
         <v>355</v>
       </c>
       <c r="F148" s="17" t="s">
@@ -6116,7 +6191,7 @@
       <c r="C149" s="66" t="n">
         <v>338</v>
       </c>
-      <c r="D149" s="67" t="n">
+      <c r="D149" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E149" s="20" t="s">
@@ -6290,13 +6365,13 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="69" t="s">
+      <c r="A158" s="68" t="s">
         <v>373</v>
       </c>
-      <c r="B158" s="70" t="n">
+      <c r="B158" s="69" t="n">
         <v>50865</v>
       </c>
-      <c r="C158" s="70" t="n">
+      <c r="C158" s="69" t="n">
         <v>51370</v>
       </c>
       <c r="D158" s="26" t="n">
@@ -6439,7 +6514,7 @@
       <c r="C165" s="66" t="n">
         <v>5158</v>
       </c>
-      <c r="D165" s="67" t="n">
+      <c r="D165" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E165" s="20" t="s">
@@ -6459,7 +6534,7 @@
       <c r="C166" s="66" t="n">
         <v>13957</v>
       </c>
-      <c r="D166" s="67" t="n">
+      <c r="D166" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E166" s="20" t="n">
@@ -6479,7 +6554,7 @@
       <c r="C167" s="66" t="n">
         <v>6544</v>
       </c>
-      <c r="D167" s="67" t="n">
+      <c r="D167" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E167" s="20" t="n">
@@ -6513,13 +6588,13 @@
       <c r="A169" s="29" t="s">
         <v>401</v>
       </c>
-      <c r="B169" s="67" t="n">
+      <c r="B169" s="37" t="n">
         <v>4560</v>
       </c>
-      <c r="C169" s="67" t="n">
+      <c r="C169" s="37" t="n">
         <v>4649</v>
       </c>
-      <c r="D169" s="67" t="n">
+      <c r="D169" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E169" s="20" t="s">
@@ -6550,16 +6625,16 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="69" t="s">
+      <c r="A171" s="68" t="s">
         <v>407</v>
       </c>
-      <c r="B171" s="67" t="n">
+      <c r="B171" s="37" t="n">
         <v>49509</v>
       </c>
-      <c r="C171" s="67" t="n">
+      <c r="C171" s="37" t="n">
         <v>51705</v>
       </c>
-      <c r="D171" s="67" t="n">
+      <c r="D171" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E171" s="20" t="s">
@@ -6570,16 +6645,16 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="71" t="s">
+      <c r="A172" s="70" t="s">
         <v>410</v>
       </c>
-      <c r="B172" s="72" t="n">
-        <v>119850</v>
-      </c>
-      <c r="C172" s="72" t="n">
-        <v>122957</v>
-      </c>
-      <c r="D172" s="72" t="n">
+      <c r="B172" s="71" t="n">
+        <v>51110</v>
+      </c>
+      <c r="C172" s="71" t="n">
+        <v>51435</v>
+      </c>
+      <c r="D172" s="71" t="n">
         <v>1</v>
       </c>
       <c r="E172" s="62" t="n">
@@ -6593,16 +6668,16 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="71" t="s">
+      <c r="A173" s="70" t="s">
         <v>410</v>
       </c>
-      <c r="B173" s="72" t="n">
-        <v>51110</v>
-      </c>
-      <c r="C173" s="72" t="n">
-        <v>51435</v>
-      </c>
-      <c r="D173" s="72" t="n">
+      <c r="B173" s="71" t="n">
+        <v>119850</v>
+      </c>
+      <c r="C173" s="71" t="n">
+        <v>122957</v>
+      </c>
+      <c r="D173" s="71" t="n">
         <v>1</v>
       </c>
       <c r="E173" s="20" t="s">
@@ -6619,13 +6694,13 @@
       <c r="A174" s="29" t="s">
         <v>413</v>
       </c>
-      <c r="B174" s="67" t="n">
+      <c r="B174" s="37" t="n">
         <v>16157</v>
       </c>
-      <c r="C174" s="67" t="n">
+      <c r="C174" s="37" t="n">
         <v>16293</v>
       </c>
-      <c r="D174" s="67" t="n">
+      <c r="D174" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E174" s="20" t="s">
@@ -6639,13 +6714,13 @@
       <c r="A175" s="29" t="s">
         <v>416</v>
       </c>
-      <c r="B175" s="67" t="n">
+      <c r="B175" s="37" t="n">
         <v>18828</v>
       </c>
-      <c r="C175" s="67" t="n">
+      <c r="C175" s="37" t="n">
         <v>19059</v>
       </c>
-      <c r="D175" s="67" t="n">
+      <c r="D175" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E175" s="20" t="s">
@@ -6659,13 +6734,13 @@
       <c r="A176" s="29" t="s">
         <v>419</v>
       </c>
-      <c r="B176" s="67" t="n">
+      <c r="B176" s="37" t="n">
         <v>18641</v>
       </c>
-      <c r="C176" s="67" t="n">
+      <c r="C176" s="37" t="n">
         <v>18836</v>
       </c>
-      <c r="D176" s="67" t="n">
+      <c r="D176" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E176" s="20" t="s">
@@ -6679,13 +6754,13 @@
       <c r="A177" s="29" t="s">
         <v>422</v>
       </c>
-      <c r="B177" s="67" t="n">
+      <c r="B177" s="37" t="n">
         <v>22091</v>
       </c>
-      <c r="C177" s="67" t="n">
+      <c r="C177" s="37" t="n">
         <v>22322</v>
       </c>
-      <c r="D177" s="67" t="n">
+      <c r="D177" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E177" s="20" t="s">
@@ -6699,13 +6774,13 @@
       <c r="A178" s="29" t="s">
         <v>425</v>
       </c>
-      <c r="B178" s="67" t="n">
+      <c r="B178" s="37" t="n">
         <v>21385</v>
       </c>
-      <c r="C178" s="67" t="n">
+      <c r="C178" s="37" t="n">
         <v>21550</v>
       </c>
-      <c r="D178" s="67" t="n">
+      <c r="D178" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E178" s="20" t="s">
@@ -6716,16 +6791,16 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="73" t="s">
+      <c r="A179" s="72" t="s">
         <v>428</v>
       </c>
-      <c r="B179" s="67" t="n">
+      <c r="B179" s="37" t="n">
         <v>37450</v>
       </c>
-      <c r="C179" s="67" t="n">
+      <c r="C179" s="37" t="n">
         <v>38151</v>
       </c>
-      <c r="D179" s="67" t="n">
+      <c r="D179" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E179" s="20" t="s">
@@ -6739,16 +6814,16 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="73" t="s">
+      <c r="A180" s="72" t="s">
         <v>428</v>
       </c>
-      <c r="B180" s="67" t="n">
+      <c r="B180" s="37" t="n">
         <v>10045</v>
       </c>
-      <c r="C180" s="67" t="n">
+      <c r="C180" s="37" t="n">
         <v>10181</v>
       </c>
-      <c r="D180" s="67" t="n">
+      <c r="D180" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E180" s="20" t="s">
@@ -6765,13 +6840,13 @@
       <c r="A181" s="29" t="s">
         <v>433</v>
       </c>
-      <c r="B181" s="67" t="n">
+      <c r="B181" s="37" t="n">
         <v>92147</v>
       </c>
-      <c r="C181" s="67" t="n">
+      <c r="C181" s="37" t="n">
         <v>93143</v>
       </c>
-      <c r="D181" s="67" t="n">
+      <c r="D181" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E181" s="20" t="s">
@@ -6785,13 +6860,13 @@
       <c r="A182" s="29" t="s">
         <v>436</v>
       </c>
-      <c r="B182" s="67" t="n">
+      <c r="B182" s="37" t="n">
         <v>42900</v>
       </c>
-      <c r="C182" s="67" t="n">
+      <c r="C182" s="37" t="n">
         <v>43348</v>
       </c>
-      <c r="D182" s="67" t="n">
+      <c r="D182" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E182" s="20" t="s">
@@ -6805,13 +6880,13 @@
       <c r="A183" s="29" t="s">
         <v>439</v>
       </c>
-      <c r="B183" s="67" t="n">
+      <c r="B183" s="37" t="n">
         <v>9640</v>
       </c>
-      <c r="C183" s="67" t="n">
+      <c r="C183" s="37" t="n">
         <v>9726</v>
       </c>
-      <c r="D183" s="67" t="n">
+      <c r="D183" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E183" s="20" t="s">
@@ -6825,13 +6900,13 @@
       <c r="A184" s="29" t="s">
         <v>442</v>
       </c>
-      <c r="B184" s="67" t="n">
+      <c r="B184" s="37" t="n">
         <v>15474</v>
       </c>
-      <c r="C184" s="67" t="n">
+      <c r="C184" s="37" t="n">
         <v>15474</v>
       </c>
-      <c r="D184" s="67" t="n">
+      <c r="D184" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E184" s="20" t="s">
@@ -6845,13 +6920,13 @@
       <c r="A185" s="29" t="s">
         <v>445</v>
       </c>
-      <c r="B185" s="67" t="n">
+      <c r="B185" s="37" t="n">
         <v>24937</v>
       </c>
-      <c r="C185" s="67" t="n">
+      <c r="C185" s="37" t="n">
         <v>25574</v>
       </c>
-      <c r="D185" s="67" t="n">
+      <c r="D185" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E185" s="20" t="s">
@@ -6865,13 +6940,13 @@
       <c r="A186" s="29" t="s">
         <v>448</v>
       </c>
-      <c r="B186" s="67" t="n">
+      <c r="B186" s="37" t="n">
         <v>14319</v>
       </c>
-      <c r="C186" s="67" t="n">
+      <c r="C186" s="37" t="n">
         <v>15243</v>
       </c>
-      <c r="D186" s="67" t="n">
+      <c r="D186" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E186" s="20" t="s">
@@ -6885,13 +6960,13 @@
       <c r="A187" s="29" t="s">
         <v>451</v>
       </c>
-      <c r="B187" s="67" t="n">
+      <c r="B187" s="37" t="n">
         <v>17358</v>
       </c>
-      <c r="C187" s="67" t="n">
+      <c r="C187" s="37" t="n">
         <v>17615</v>
       </c>
-      <c r="D187" s="67" t="n">
+      <c r="D187" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E187" s="20" t="s">
@@ -6905,13 +6980,13 @@
       <c r="A188" s="29" t="s">
         <v>454</v>
       </c>
-      <c r="B188" s="67" t="n">
+      <c r="B188" s="37" t="n">
         <v>46075</v>
       </c>
-      <c r="C188" s="67" t="n">
+      <c r="C188" s="37" t="n">
         <v>46343</v>
       </c>
-      <c r="D188" s="67" t="n">
+      <c r="D188" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E188" s="20" t="s">
@@ -6925,13 +7000,13 @@
       <c r="A189" s="29" t="s">
         <v>457</v>
       </c>
-      <c r="B189" s="67" t="n">
+      <c r="B189" s="37" t="n">
         <v>24773</v>
       </c>
-      <c r="C189" s="67" t="n">
+      <c r="C189" s="37" t="n">
         <v>25111</v>
       </c>
-      <c r="D189" s="67" t="n">
+      <c r="D189" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E189" s="20" t="s">
@@ -6945,13 +7020,13 @@
       <c r="A190" s="29" t="s">
         <v>460</v>
       </c>
-      <c r="B190" s="67" t="n">
+      <c r="B190" s="37" t="n">
         <v>36173</v>
       </c>
-      <c r="C190" s="67" t="n">
+      <c r="C190" s="37" t="n">
         <v>36546</v>
       </c>
-      <c r="D190" s="67" t="n">
+      <c r="D190" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E190" s="20" t="s">
@@ -6965,13 +7040,13 @@
       <c r="A191" s="29" t="s">
         <v>463</v>
       </c>
-      <c r="B191" s="74" t="n">
+      <c r="B191" s="73" t="n">
         <v>66445</v>
       </c>
-      <c r="C191" s="74" t="n">
+      <c r="C191" s="73" t="n">
         <v>66445</v>
       </c>
-      <c r="D191" s="67" t="n">
+      <c r="D191" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E191" s="20" t="s">
@@ -6985,13 +7060,13 @@
       <c r="A192" s="29" t="s">
         <v>466</v>
       </c>
-      <c r="B192" s="67" t="n">
-        <v>60945</v>
-      </c>
-      <c r="C192" s="67" t="n">
-        <v>61833</v>
-      </c>
-      <c r="D192" s="67" t="n">
+      <c r="B192" s="25" t="n">
+        <v>76705</v>
+      </c>
+      <c r="C192" s="25" t="n">
+        <v>77913</v>
+      </c>
+      <c r="D192" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E192" s="20" t="s">
@@ -7005,11 +7080,11 @@
       <c r="A193" s="29" t="s">
         <v>469</v>
       </c>
-      <c r="B193" s="25" t="n">
-        <v>76705</v>
-      </c>
-      <c r="C193" s="25" t="n">
-        <v>77913</v>
+      <c r="B193" s="37" t="n">
+        <v>60945</v>
+      </c>
+      <c r="C193" s="37" t="n">
+        <v>61833</v>
       </c>
       <c r="D193" s="25" t="n">
         <v>1</v>
@@ -7025,13 +7100,13 @@
       <c r="A194" s="29" t="s">
         <v>472</v>
       </c>
-      <c r="B194" s="67" t="n">
+      <c r="B194" s="37" t="n">
         <v>46237</v>
       </c>
-      <c r="C194" s="67" t="n">
+      <c r="C194" s="37" t="n">
         <v>47733</v>
       </c>
-      <c r="D194" s="67" t="n">
+      <c r="D194" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E194" s="20" t="s">
@@ -7045,13 +7120,13 @@
       <c r="A195" s="29" t="s">
         <v>475</v>
       </c>
-      <c r="B195" s="67" t="n">
+      <c r="B195" s="37" t="n">
         <v>56994</v>
       </c>
-      <c r="C195" s="67" t="n">
+      <c r="C195" s="37" t="n">
         <v>57578</v>
       </c>
-      <c r="D195" s="67" t="n">
+      <c r="D195" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E195" s="20" t="s">
@@ -7065,13 +7140,13 @@
       <c r="A196" s="29" t="s">
         <v>478</v>
       </c>
-      <c r="B196" s="67" t="n">
+      <c r="B196" s="37" t="n">
         <v>180061</v>
       </c>
-      <c r="C196" s="67" t="n">
+      <c r="C196" s="37" t="n">
         <v>180914</v>
       </c>
-      <c r="D196" s="67" t="n">
+      <c r="D196" s="37" t="n">
         <v>1</v>
       </c>
       <c r="E196" s="20" t="s">
@@ -7182,14 +7257,14 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="71" t="s">
+      <c r="A202" s="70" t="s">
         <v>496</v>
       </c>
       <c r="B202" s="25" t="n">
-        <v>27245</v>
+        <v>36408</v>
       </c>
       <c r="C202" s="25" t="n">
-        <v>29028</v>
+        <v>37965</v>
       </c>
       <c r="D202" s="26" t="n">
         <v>1</v>
@@ -7205,14 +7280,14 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="71" t="s">
+      <c r="A203" s="70" t="s">
         <v>496</v>
       </c>
       <c r="B203" s="25" t="n">
-        <v>36408</v>
+        <v>27245</v>
       </c>
       <c r="C203" s="25" t="n">
-        <v>37965</v>
+        <v>29028</v>
       </c>
       <c r="D203" s="26" t="n">
         <v>1</v>
@@ -7267,46 +7342,47 @@
         <v>505</v>
       </c>
     </row>
+    <row r="206" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="24" t="s">
+        <v>506</v>
+      </c>
+      <c r="B206" s="25" t="n">
+        <v>44725</v>
+      </c>
+      <c r="C206" s="25" t="n">
+        <v>47195</v>
+      </c>
+      <c r="D206" s="74" t="n">
+        <v>1</v>
+      </c>
+      <c r="E206" s="20" t="n">
+        <v>3275</v>
+      </c>
+      <c r="F206" s="17" t="s">
+        <v>507</v>
+      </c>
+    </row>
     <row r="207" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="75" t="s">
-        <v>506</v>
+      <c r="A207" s="24" t="s">
+        <v>508</v>
       </c>
       <c r="B207" s="25" t="n">
-        <v>44725</v>
+        <v>188294</v>
       </c>
       <c r="C207" s="25" t="n">
-        <v>47195</v>
-      </c>
-      <c r="D207" s="76" t="n">
+        <v>189525</v>
+      </c>
+      <c r="D207" s="26" t="n">
         <v>1</v>
       </c>
       <c r="E207" s="20" t="n">
-        <v>3275</v>
+        <v>3868</v>
       </c>
       <c r="F207" s="17" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="75" t="s">
-        <v>508</v>
-      </c>
-      <c r="B208" s="25" t="n">
-        <v>188294</v>
-      </c>
-      <c r="C208" s="25" t="n">
-        <v>189525</v>
-      </c>
-      <c r="D208" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E208" s="20" t="n">
-        <v>3868</v>
-      </c>
-      <c r="F208" s="17" t="s">
         <v>509</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -7316,4 +7392,534 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J34"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="39.45"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="75" t="s">
+        <v>510</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>511</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1" s="76"/>
+      <c r="E1" s="77" t="s">
+        <v>513</v>
+      </c>
+      <c r="F1" s="77"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+    </row>
+    <row r="2" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="76" t="s">
+        <v>514</v>
+      </c>
+      <c r="D2" s="76" t="s">
+        <v>515</v>
+      </c>
+      <c r="E2" s="77" t="s">
+        <v>514</v>
+      </c>
+      <c r="F2" s="77" t="s">
+        <v>515</v>
+      </c>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+    </row>
+    <row r="3" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="s">
+        <v>467</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>468</v>
+      </c>
+      <c r="C3" s="78" t="n">
+        <v>76705</v>
+      </c>
+      <c r="D3" s="78" t="n">
+        <v>77913</v>
+      </c>
+      <c r="E3" s="79" t="n">
+        <v>60945</v>
+      </c>
+      <c r="F3" s="79" t="n">
+        <v>61833</v>
+      </c>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+    </row>
+    <row r="4" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="20" t="s">
+        <v>470</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>471</v>
+      </c>
+      <c r="C4" s="80" t="n">
+        <v>60945</v>
+      </c>
+      <c r="D4" s="80" t="n">
+        <v>61833</v>
+      </c>
+      <c r="E4" s="81" t="n">
+        <v>76705</v>
+      </c>
+      <c r="F4" s="81" t="n">
+        <v>77913</v>
+      </c>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+    </row>
+    <row r="5" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+    </row>
+    <row r="6" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="20" t="s">
+        <v>497</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>498</v>
+      </c>
+      <c r="C6" s="78" t="n">
+        <v>36408</v>
+      </c>
+      <c r="D6" s="78" t="n">
+        <v>37965</v>
+      </c>
+      <c r="E6" s="81" t="n">
+        <v>27245</v>
+      </c>
+      <c r="F6" s="81" t="n">
+        <v>29028</v>
+      </c>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+    </row>
+    <row r="7" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="20" t="s">
+        <v>499</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>498</v>
+      </c>
+      <c r="C7" s="78" t="n">
+        <v>27245</v>
+      </c>
+      <c r="D7" s="78" t="n">
+        <v>29028</v>
+      </c>
+      <c r="E7" s="81" t="n">
+        <v>36408</v>
+      </c>
+      <c r="F7" s="81" t="n">
+        <v>37965</v>
+      </c>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+    </row>
+    <row r="8" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+    </row>
+    <row r="9" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="62" t="n">
+        <v>3855</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="C9" s="86" t="n">
+        <v>51110</v>
+      </c>
+      <c r="D9" s="86" t="n">
+        <v>51435</v>
+      </c>
+      <c r="E9" s="87" t="n">
+        <v>119850</v>
+      </c>
+      <c r="F9" s="87" t="n">
+        <v>122957</v>
+      </c>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+    </row>
+    <row r="10" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="C10" s="86" t="n">
+        <v>119850</v>
+      </c>
+      <c r="D10" s="86" t="n">
+        <v>122957</v>
+      </c>
+      <c r="E10" s="87" t="n">
+        <v>51110</v>
+      </c>
+      <c r="F10" s="87" t="n">
+        <v>51435</v>
+      </c>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+    </row>
+    <row r="11" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="74"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+    </row>
+    <row r="12" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="74"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
+    </row>
+    <row r="13" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="74"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+    </row>
+    <row r="14" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+    </row>
+    <row r="15" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="74"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+    </row>
+    <row r="16" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="74"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+    </row>
+    <row r="17" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="74"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+    </row>
+    <row r="18" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="74"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="74"/>
+    </row>
+    <row r="19" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="74"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="74"/>
+    </row>
+    <row r="20" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="74"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
+    </row>
+    <row r="21" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="74"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+    </row>
+    <row r="22" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="74"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+    </row>
+    <row r="23" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="74"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+    </row>
+    <row r="24" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="74"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+    </row>
+    <row r="25" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="74"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="74"/>
+    </row>
+    <row r="26" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="74"/>
+      <c r="B26" s="74"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+    </row>
+    <row r="27" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="74"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+    </row>
+    <row r="28" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="74"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
+    </row>
+    <row r="29" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="74"/>
+      <c r="B29" s="74"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="74"/>
+    </row>
+    <row r="30" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="74"/>
+      <c r="B30" s="74"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+    </row>
+    <row r="31" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="74"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
+    </row>
+    <row r="32" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="74"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="74"/>
+    </row>
+    <row r="33" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="74"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+    </row>
+    <row r="34" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="74"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>